<commit_message>
RRH-4057: Fjernet orgform ESEK fra kodeverk excel-fil for maskinell innrapportering
</commit_message>
<xml_diff>
--- a/content/apidokumentasjon/reelle-rettighetshavere/maskinell-innrapportering/beskrivelse-av-felter/Kodeverk MINN.xlsx
+++ b/content/apidokumentasjon/reelle-rettighetshavere/maskinell-innrapportering/beskrivelse-av-felter/Kodeverk MINN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28104"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://registrene-my.sharepoint.com/personal/ata_brreg_no/Documents/Skrivebord/Reelle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="421" documentId="8_{A6C3059F-C635-4164-9987-8DAB11CCA571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67522DD6-698A-418A-8505-6CD22AE5B5F7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AA75B45-48F5-48EF-B168-2F6ED1EFFCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" xr2:uid="{8B48753F-9CAB-42E5-B3FE-117B54C8CFC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{8B48753F-9CAB-42E5-B3FE-117B54C8CFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="ReelleRettighetshavereidentifik" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="131">
   <si>
     <t>kode</t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>SE</t>
-  </si>
-  <si>
-    <t>ESEK</t>
   </si>
   <si>
     <t>ANS</t>
@@ -1492,7 +1489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63993C0A-FCA1-4A31-A746-1ABE8E19AF72}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1630,31 +1627,31 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -1662,10 +1659,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -1673,10 +1670,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -1684,10 +1681,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -1695,10 +1692,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -1706,10 +1703,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>125</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -2520,10 +2517,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F088584E-11E9-4B62-A8D6-2CE5D935642A}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2786,8 +2783,8 @@
       <c r="B14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>93</v>
+      <c r="C14" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>93</v>
@@ -2805,8 +2802,8 @@
       <c r="B15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>96</v>
+      <c r="C15" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>93</v>
@@ -2837,17 +2834,17 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>93</v>
+      <c r="B17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="22"/>
@@ -2865,8 +2862,8 @@
       <c r="C18" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>96</v>
+      <c r="D18" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="22"/>
@@ -2893,29 +2890,10 @@
       <c r="I19" s="22"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="9"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F2:F20"/>
-    <mergeCell ref="G2:I20"/>
+    <mergeCell ref="F2:F19"/>
+    <mergeCell ref="G2:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2923,10 +2901,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782C364C-B661-4E2D-A1DF-C2CFF9423646}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B69" sqref="B66:B69"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2935,329 +2913,313 @@
     <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>117</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>92</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="12" t="s">
         <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="B14" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="5" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="12" t="s">
         <v>99</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="12" t="s">
         <v>100</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3265,7 +3227,7 @@
         <v>102</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3273,7 +3235,7 @@
         <v>103</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3281,7 +3243,7 @@
         <v>103</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3289,7 +3251,7 @@
         <v>103</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3297,7 +3259,7 @@
         <v>103</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3305,7 +3267,7 @@
         <v>104</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3313,7 +3275,7 @@
         <v>104</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3321,7 +3283,7 @@
         <v>104</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3329,7 +3291,7 @@
         <v>104</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3337,7 +3299,7 @@
         <v>105</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3345,7 +3307,7 @@
         <v>105</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3353,7 +3315,7 @@
         <v>105</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3361,7 +3323,7 @@
         <v>105</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3369,7 +3331,7 @@
         <v>106</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3377,7 +3339,7 @@
         <v>106</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3385,7 +3347,7 @@
         <v>106</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3393,7 +3355,7 @@
         <v>106</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3401,7 +3363,7 @@
         <v>107</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3409,7 +3371,7 @@
         <v>107</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3417,7 +3379,7 @@
         <v>107</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3425,7 +3387,7 @@
         <v>107</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3433,7 +3395,7 @@
         <v>108</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3441,7 +3403,7 @@
         <v>108</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3449,7 +3411,7 @@
         <v>108</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3457,7 +3419,7 @@
         <v>108</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3465,7 +3427,7 @@
         <v>109</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3473,7 +3435,7 @@
         <v>109</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3481,7 +3443,7 @@
         <v>109</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3489,144 +3451,112 @@
         <v>109</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="13"/>
-      <c r="B78" s="10"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:H16"/>
+    <mergeCell ref="E2:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3648,13 +3578,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>127</v>
       </c>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
@@ -3663,7 +3593,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>82</v>
@@ -3676,7 +3606,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>84</v>
@@ -3689,7 +3619,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>86</v>
@@ -3702,7 +3632,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>82</v>
@@ -3715,7 +3645,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>84</v>
@@ -3728,7 +3658,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>86</v>
@@ -3794,13 +3724,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>129</v>
       </c>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
@@ -3808,7 +3738,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>75</v>
@@ -3820,7 +3750,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>77</v>
@@ -3832,7 +3762,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>75</v>
@@ -3844,7 +3774,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>77</v>
@@ -3856,7 +3786,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>79</v>
@@ -3868,7 +3798,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
RRH-4057: Fjernet orgform ESEK fra siden "test og produksjon" og kodeverk for maskinell innrapportering (#58)
</commit_message>
<xml_diff>
--- a/content/apidokumentasjon/reelle-rettighetshavere/maskinell-innrapportering/beskrivelse-av-felter/Kodeverk MINN.xlsx
+++ b/content/apidokumentasjon/reelle-rettighetshavere/maskinell-innrapportering/beskrivelse-av-felter/Kodeverk MINN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28104"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://registrene-my.sharepoint.com/personal/ata_brreg_no/Documents/Skrivebord/Reelle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="421" documentId="8_{A6C3059F-C635-4164-9987-8DAB11CCA571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67522DD6-698A-418A-8505-6CD22AE5B5F7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AA75B45-48F5-48EF-B168-2F6ED1EFFCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" xr2:uid="{8B48753F-9CAB-42E5-B3FE-117B54C8CFC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{8B48753F-9CAB-42E5-B3FE-117B54C8CFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="ReelleRettighetshavereidentifik" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="131">
   <si>
     <t>kode</t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>SE</t>
-  </si>
-  <si>
-    <t>ESEK</t>
   </si>
   <si>
     <t>ANS</t>
@@ -1492,7 +1489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63993C0A-FCA1-4A31-A746-1ABE8E19AF72}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1630,31 +1627,31 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -1662,10 +1659,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -1673,10 +1670,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -1684,10 +1681,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -1695,10 +1692,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -1706,10 +1703,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>125</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -2520,10 +2517,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F088584E-11E9-4B62-A8D6-2CE5D935642A}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2786,8 +2783,8 @@
       <c r="B14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>93</v>
+      <c r="C14" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>93</v>
@@ -2805,8 +2802,8 @@
       <c r="B15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>96</v>
+      <c r="C15" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>93</v>
@@ -2837,17 +2834,17 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>93</v>
+      <c r="B17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="22"/>
@@ -2865,8 +2862,8 @@
       <c r="C18" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>96</v>
+      <c r="D18" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="22"/>
@@ -2893,29 +2890,10 @@
       <c r="I19" s="22"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="9"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F2:F20"/>
-    <mergeCell ref="G2:I20"/>
+    <mergeCell ref="F2:F19"/>
+    <mergeCell ref="G2:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2923,10 +2901,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782C364C-B661-4E2D-A1DF-C2CFF9423646}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B69" sqref="B66:B69"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2935,329 +2913,313 @@
     <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>117</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>92</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="12" t="s">
         <v>95</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="B14" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="5" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="12" t="s">
         <v>99</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="12" t="s">
         <v>100</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3265,7 +3227,7 @@
         <v>102</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3273,7 +3235,7 @@
         <v>103</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3281,7 +3243,7 @@
         <v>103</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3289,7 +3251,7 @@
         <v>103</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3297,7 +3259,7 @@
         <v>103</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3305,7 +3267,7 @@
         <v>104</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3313,7 +3275,7 @@
         <v>104</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3321,7 +3283,7 @@
         <v>104</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3329,7 +3291,7 @@
         <v>104</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3337,7 +3299,7 @@
         <v>105</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3345,7 +3307,7 @@
         <v>105</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3353,7 +3315,7 @@
         <v>105</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3361,7 +3323,7 @@
         <v>105</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3369,7 +3331,7 @@
         <v>106</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3377,7 +3339,7 @@
         <v>106</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3385,7 +3347,7 @@
         <v>106</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3393,7 +3355,7 @@
         <v>106</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3401,7 +3363,7 @@
         <v>107</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3409,7 +3371,7 @@
         <v>107</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3417,7 +3379,7 @@
         <v>107</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3425,7 +3387,7 @@
         <v>107</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3433,7 +3395,7 @@
         <v>108</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3441,7 +3403,7 @@
         <v>108</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3449,7 +3411,7 @@
         <v>108</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3457,7 +3419,7 @@
         <v>108</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3465,7 +3427,7 @@
         <v>109</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3473,7 +3435,7 @@
         <v>109</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3481,7 +3443,7 @@
         <v>109</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3489,144 +3451,112 @@
         <v>109</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="13"/>
-      <c r="B78" s="10"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:H16"/>
+    <mergeCell ref="E2:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3648,13 +3578,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>127</v>
       </c>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
@@ -3663,7 +3593,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>82</v>
@@ -3676,7 +3606,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>84</v>
@@ -3689,7 +3619,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>86</v>
@@ -3702,7 +3632,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>82</v>
@@ -3715,7 +3645,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>84</v>
@@ -3728,7 +3658,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>86</v>
@@ -3794,13 +3724,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>129</v>
       </c>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
@@ -3808,7 +3738,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>75</v>
@@ -3820,7 +3750,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>77</v>
@@ -3832,7 +3762,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>75</v>
@@ -3844,7 +3774,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>77</v>
@@ -3856,7 +3786,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>79</v>
@@ -3868,7 +3798,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>79</v>

</xml_diff>